<commit_message>
Switch to get_dPower_WeightsK from InOutModule
Move example-file for database to InOutModule
Adjust example to new format
</commit_message>
<xml_diff>
--- a/data/example/Power_WeightsK.xlsx
+++ b/data/example/Power_WeightsK.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Nextcloud/lego_africa/Arbeit/06_Projekte/2024/LEGO Datenbank/Output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D641E1B-F512-4449-B80E-8DFA84630079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5438F227-2DA6-4B0D-A1BC-350A61FDF5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="687" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Power Weights K" sheetId="58" r:id="rId1"/>
+    <sheet name="ScenarioA" sheetId="58" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="businfo">#REF!</definedName>
@@ -39,25 +39,14 @@
     <definedName name="sCodeName">#REF!</definedName>
     <definedName name="storage">#REF!</definedName>
     <definedName name="thermalgen">#REF!</definedName>
-    <definedName name="weight_k">'Power Weights K'!$B$5:$E$32</definedName>
+    <definedName name="weight_k">ScenarioA!$B$5:$E$33</definedName>
     <definedName name="weight_rp">#REF!</definedName>
     <definedName name="zones">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <customWorkbookViews>
     <customWorkbookView name="Andres Ramos - Vista personalizada" guid="{162D0EED-4A71-4EB6-8FDF-A42498BFDBC9}" autoUpdate="1" mergeInterval="5" onlySync="1" personalView="1" maximized="1" windowWidth="1112" windowHeight="624" tabRatio="506" activeSheetId="1"/>
   </customWorkbookViews>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -67,23 +56,39 @@
     <author>Felix Auer</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{FCC0D290-893B-4843-B1D8-FED29AB6B79B}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Hours K</t>
+          <t>Readable Name</t>
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{4AB0AACC-F7F1-4128-A02F-BB094CCF3A09}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value specifier in DB</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
@@ -93,16 +98,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{CCEA2CE9-31D5-4FD8-B9BD-B49D8B1D8127}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
+            <b/>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Source/ Typical Values</t>
+          <t>Details on database behavior</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit or valid values</t>
         </r>
       </text>
     </comment>
@@ -111,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
   <si>
     <t>k0001</t>
   </si>
@@ -185,9 +205,6 @@
     <t>k0024</t>
   </si>
   <si>
-    <t>pWeight_k(k)</t>
-  </si>
-  <si>
     <t>hourly weight for each rp</t>
   </si>
   <si>
@@ -195,13 +212,85 @@
   </si>
   <si>
     <t>Power - Weights K</t>
+  </si>
+  <si>
+    <t>Format:</t>
+  </si>
+  <si>
+    <t>Database ID</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ID within database</t>
+  </si>
+  <si>
+    <t>Filled automatically by database</t>
+  </si>
+  <si>
+    <t>[db-key]</t>
+  </si>
+  <si>
+    <t>Data Package</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t>dataPackage</t>
+  </si>
+  <si>
+    <t>dataSource</t>
+  </si>
+  <si>
+    <t>Where the data for the entry comes from</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[DataPackage]</t>
+  </si>
+  <si>
+    <t>[DataSource]</t>
+  </si>
+  <si>
+    <t>TestPackage1</t>
+  </si>
+  <si>
+    <t>TestSource1</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Hour within representative period</t>
+  </si>
+  <si>
+    <t>[k]</t>
+  </si>
+  <si>
+    <t>Weight of hour k within representative period</t>
+  </si>
+  <si>
+    <t>Which package this belongs to</t>
+  </si>
+  <si>
+    <t>Scenario-dependent</t>
+  </si>
+  <si>
+    <t>pWeight_k</t>
+  </si>
+  <si>
+    <t>v0.0.2r</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -242,59 +331,51 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <name val="Aptos"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
       <name val="Aptos"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Aptos"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Aptos"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color theme="0"/>
       <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +423,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -367,7 +460,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -378,47 +471,61 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
-    <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
-    <cellStyle name="Link" xfId="8" builtinId="8"/>
-    <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
-    <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+  <cellStyles count="8">
+    <cellStyle name="Data" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Hervorhebung" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Standard 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -733,268 +840,491 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja14">
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:E31"/>
+  <dimension ref="B1:F32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E1" sqref="E1:F1048576"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1:F1048576"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:F1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="11.3984375" style="2"/>
+    <col min="2" max="2" width="16.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="26" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="2:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C3" s="3" t="s">
+      <c r="C2" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="E7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="8">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8">
-        <v>1</v>
-      </c>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
+      <c r="D13" s="16">
+        <v>1</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="8">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="16">
+        <v>1</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="8">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="8">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="8">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="16">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="8">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="8">
-        <v>1</v>
-      </c>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="8">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
+      <c r="D20" s="16">
+        <v>1</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="8">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="16">
+        <v>1</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="8">
-        <v>1</v>
-      </c>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
+      <c r="D22" s="16">
+        <v>1</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="8">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
+      <c r="D23" s="16">
+        <v>1</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="8">
-        <v>1</v>
-      </c>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
+      <c r="D24" s="16">
+        <v>1</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="12"/>
+      <c r="C25" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="8">
-        <v>1</v>
-      </c>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
+      <c r="D25" s="16">
+        <v>1</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="12"/>
+      <c r="C26" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="8">
-        <v>1</v>
-      </c>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
+      <c r="D26" s="16">
+        <v>1</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="12"/>
+      <c r="C27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="8">
-        <v>1</v>
-      </c>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
+      <c r="D27" s="16">
+        <v>1</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="12"/>
+      <c r="C28" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="8">
-        <v>1</v>
-      </c>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
+      <c r="D28" s="16">
+        <v>1</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="12"/>
+      <c r="C29" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="8">
-        <v>1</v>
-      </c>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="2" t="s">
+      <c r="D29" s="16">
+        <v>1</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="12"/>
+      <c r="C30" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="8">
-        <v>1</v>
-      </c>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="2" t="s">
+      <c r="D30" s="16">
+        <v>1</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="12"/>
+      <c r="C31" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="8">
-        <v>1</v>
-      </c>
-      <c r="D30" s="6"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="7"/>
-      <c r="E31" s="6"/>
+      <c r="D31" s="16">
+        <v>1</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="E32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -1005,6 +1335,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1013,7 +1349,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1159,13 +1495,23 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1173,7 +1519,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1189,20 +1535,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>